<commit_message>
dropping health notes as a field
</commit_message>
<xml_diff>
--- a/disease_data_template.xlsx
+++ b/disease_data_template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Live capture </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health notes</t>
   </si>
   <si>
     <t xml:space="preserve">Host life stage</t>
@@ -157,6 +154,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -241,24 +239,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,168 +449,166 @@
   </sheetPr>
   <dimension ref="A1:AO1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="15.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="24" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="15.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="29" style="0" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="32" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="20.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="24.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="15.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="4.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="8.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="5.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="1" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="15.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="28" style="1" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="31" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="20.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="24.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="38" style="1" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="17.44"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AO1" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>